<commit_message>
HP and LP column
</commit_message>
<xml_diff>
--- a/Track.xlsx
+++ b/Track.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Files\Code\Tracker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7820996B-4FC8-4ACD-A78D-C028F77A4C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC68AE3-B490-4B9F-AEAB-5BAEE0075C71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4476CF2B-F9B1-450A-BDD4-217B8772DEDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4476CF2B-F9B1-450A-BDD4-217B8772DEDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="46">
   <si>
     <t>C0</t>
   </si>
@@ -167,6 +167,12 @@
   </si>
   <si>
     <t>Vol</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>LP</t>
   </si>
 </sst>
 </file>
@@ -1252,9 +1258,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:BJ133"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H21" sqref="B6:H21"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AO17" sqref="AO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,65 +1832,89 @@
       <c r="H5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="13"/>
-      <c r="J5" s="9" t="s">
+      <c r="I5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="13"/>
+      <c r="L5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9" t="s">
+      <c r="M5" s="9"/>
+      <c r="N5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="O5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="P5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="Q5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="P5" s="14" t="s">
+      <c r="R5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Q5" s="9"/>
-      <c r="R5" s="9" t="s">
+      <c r="S5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="T5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="U5" s="13"/>
+      <c r="V5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="9"/>
-      <c r="T5" s="9" t="s">
+      <c r="W5" s="9"/>
+      <c r="X5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="Y5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="V5" s="9" t="s">
+      <c r="Z5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="W5" s="9" t="s">
+      <c r="AA5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="9" t="s">
+      <c r="AB5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="9" t="s">
+      <c r="AC5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD5" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="AA5" s="9"/>
-      <c r="AB5" s="9" t="s">
+      <c r="AG5" s="9"/>
+      <c r="AH5" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="AC5" s="9" t="s">
+      <c r="AI5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="AD5" s="9" t="s">
+      <c r="AJ5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="AE5" s="9" t="s">
+      <c r="AK5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="AF5" s="14" t="s">
+      <c r="AL5" s="9" t="s">
         <v>26</v>
+      </c>
+      <c r="AM5" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="AN5" s="14" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1899,33 +1929,41 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="15">
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="15">
         <v>65</v>
       </c>
-      <c r="J6" s="3"/>
       <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="16"/>
-      <c r="Q6" s="2">
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="2">
         <v>129</v>
       </c>
-      <c r="R6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
       <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
       <c r="X6" s="3"/>
-      <c r="Y6" s="15">
-        <v>193</v>
-      </c>
+      <c r="Y6" s="3"/>
       <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="16"/>
+      <c r="AE6" s="15">
+        <v>193</v>
+      </c>
+      <c r="AF6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="16"/>
     </row>
     <row r="7" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
@@ -1937,33 +1975,41 @@
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="I7" s="15">
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="15">
         <v>66</v>
       </c>
-      <c r="J7" s="3"/>
       <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="2">
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="2">
         <v>130</v>
       </c>
-      <c r="R7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
       <c r="X7" s="3"/>
-      <c r="Y7" s="15">
-        <v>194</v>
-      </c>
+      <c r="Y7" s="3"/>
       <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="16"/>
+      <c r="AE7" s="15">
+        <v>194</v>
+      </c>
+      <c r="AF7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="16"/>
     </row>
     <row r="8" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
@@ -1975,33 +2021,41 @@
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="I8" s="15">
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="15">
         <v>67</v>
       </c>
-      <c r="J8" s="3"/>
       <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="2">
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="2">
         <v>131</v>
       </c>
-      <c r="R8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
       <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
       <c r="X8" s="3"/>
-      <c r="Y8" s="15">
-        <v>195</v>
-      </c>
+      <c r="Y8" s="3"/>
       <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="16"/>
+      <c r="AE8" s="15">
+        <v>195</v>
+      </c>
+      <c r="AF8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="16"/>
     </row>
     <row r="9" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
@@ -2013,33 +2067,41 @@
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
-      <c r="I9" s="15">
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="15">
         <v>68</v>
       </c>
-      <c r="J9" s="3"/>
       <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
       <c r="N9" s="3"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="16"/>
-      <c r="Q9" s="2">
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="16"/>
+      <c r="U9" s="2">
         <v>132</v>
       </c>
-      <c r="R9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
       <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
       <c r="X9" s="3"/>
-      <c r="Y9" s="15">
-        <v>196</v>
-      </c>
+      <c r="Y9" s="3"/>
       <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="16"/>
+      <c r="AE9" s="15">
+        <v>196</v>
+      </c>
+      <c r="AF9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="16"/>
     </row>
     <row r="10" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
@@ -2051,33 +2113,41 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="17">
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="17">
         <v>69</v>
       </c>
-      <c r="J10" s="3"/>
       <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
       <c r="N10" s="3"/>
       <c r="O10" s="3"/>
-      <c r="P10" s="16"/>
-      <c r="Q10" s="11">
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="16"/>
+      <c r="U10" s="11">
         <v>133</v>
       </c>
-      <c r="R10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
       <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
       <c r="X10" s="3"/>
-      <c r="Y10" s="17">
-        <v>197</v>
-      </c>
+      <c r="Y10" s="3"/>
       <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="16"/>
+      <c r="AE10" s="17">
+        <v>197</v>
+      </c>
+      <c r="AF10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="16"/>
     </row>
     <row r="11" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17">
@@ -2089,33 +2159,41 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
-      <c r="I11" s="17">
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="17">
         <v>70</v>
       </c>
-      <c r="J11" s="3"/>
       <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
       <c r="N11" s="3"/>
       <c r="O11" s="3"/>
-      <c r="P11" s="16"/>
-      <c r="Q11" s="11">
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="16"/>
+      <c r="U11" s="11">
         <v>134</v>
       </c>
-      <c r="R11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
       <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
       <c r="X11" s="3"/>
-      <c r="Y11" s="17">
-        <v>198</v>
-      </c>
+      <c r="Y11" s="3"/>
       <c r="Z11" s="3"/>
+      <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
-      <c r="AF11" s="16"/>
+      <c r="AE11" s="17">
+        <v>198</v>
+      </c>
+      <c r="AF11" s="3"/>
+      <c r="AH11" s="3"/>
+      <c r="AI11" s="3"/>
+      <c r="AJ11" s="3"/>
+      <c r="AK11" s="3"/>
+      <c r="AL11" s="3"/>
+      <c r="AM11" s="3"/>
+      <c r="AN11" s="16"/>
     </row>
     <row r="12" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
@@ -2127,33 +2205,41 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
-      <c r="I12" s="17">
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="17">
         <v>71</v>
       </c>
-      <c r="J12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
       <c r="N12" s="3"/>
       <c r="O12" s="3"/>
-      <c r="P12" s="16"/>
-      <c r="Q12" s="11">
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="16"/>
+      <c r="U12" s="11">
         <v>135</v>
       </c>
-      <c r="R12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
       <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
       <c r="X12" s="3"/>
-      <c r="Y12" s="17">
-        <v>199</v>
-      </c>
+      <c r="Y12" s="3"/>
       <c r="Z12" s="3"/>
+      <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="16"/>
+      <c r="AE12" s="17">
+        <v>199</v>
+      </c>
+      <c r="AF12" s="3"/>
+      <c r="AH12" s="3"/>
+      <c r="AI12" s="3"/>
+      <c r="AJ12" s="3"/>
+      <c r="AK12" s="3"/>
+      <c r="AL12" s="3"/>
+      <c r="AM12" s="3"/>
+      <c r="AN12" s="16"/>
     </row>
     <row r="13" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17">
@@ -2165,33 +2251,41 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="17">
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="17">
         <v>72</v>
       </c>
-      <c r="J13" s="3"/>
       <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="11">
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="16"/>
+      <c r="U13" s="11">
         <v>136</v>
       </c>
-      <c r="R13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
       <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
       <c r="X13" s="3"/>
-      <c r="Y13" s="17">
-        <v>200</v>
-      </c>
+      <c r="Y13" s="3"/>
       <c r="Z13" s="3"/>
+      <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="16"/>
+      <c r="AE13" s="17">
+        <v>200</v>
+      </c>
+      <c r="AF13" s="3"/>
+      <c r="AH13" s="3"/>
+      <c r="AI13" s="3"/>
+      <c r="AJ13" s="3"/>
+      <c r="AK13" s="3"/>
+      <c r="AL13" s="3"/>
+      <c r="AM13" s="3"/>
+      <c r="AN13" s="16"/>
     </row>
     <row r="14" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
@@ -2203,33 +2297,41 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
-      <c r="I14" s="15">
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="15">
         <v>73</v>
       </c>
-      <c r="J14" s="3"/>
       <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
       <c r="N14" s="3"/>
       <c r="O14" s="3"/>
-      <c r="P14" s="16"/>
-      <c r="Q14" s="2">
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="16"/>
+      <c r="U14" s="2">
         <v>137</v>
       </c>
-      <c r="R14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
       <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
       <c r="X14" s="3"/>
-      <c r="Y14" s="15">
-        <v>201</v>
-      </c>
+      <c r="Y14" s="3"/>
       <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="16"/>
+      <c r="AE14" s="15">
+        <v>201</v>
+      </c>
+      <c r="AF14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="16"/>
     </row>
     <row r="15" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
@@ -2241,33 +2343,41 @@
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
-      <c r="I15" s="15">
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="15">
         <v>74</v>
       </c>
-      <c r="J15" s="3"/>
       <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
       <c r="N15" s="3"/>
       <c r="O15" s="3"/>
-      <c r="P15" s="16"/>
-      <c r="Q15" s="2">
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="16"/>
+      <c r="U15" s="2">
         <v>138</v>
       </c>
-      <c r="R15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
       <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
       <c r="X15" s="3"/>
-      <c r="Y15" s="15">
-        <v>202</v>
-      </c>
+      <c r="Y15" s="3"/>
       <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="16"/>
+      <c r="AE15" s="15">
+        <v>202</v>
+      </c>
+      <c r="AF15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="16"/>
     </row>
     <row r="16" spans="1:62" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
@@ -2279,35 +2389,43 @@
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
-      <c r="I16" s="15">
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="15">
         <v>75</v>
       </c>
-      <c r="J16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
       <c r="N16" s="3"/>
       <c r="O16" s="3"/>
-      <c r="P16" s="16"/>
-      <c r="Q16" s="2">
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3"/>
+      <c r="T16" s="16"/>
+      <c r="U16" s="2">
         <v>139</v>
       </c>
-      <c r="R16" s="3"/>
-      <c r="T16" s="3"/>
-      <c r="U16" s="3"/>
       <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
       <c r="X16" s="3"/>
-      <c r="Y16" s="15">
-        <v>203</v>
-      </c>
+      <c r="Y16" s="3"/>
       <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="16"/>
-    </row>
-    <row r="17" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE16" s="15">
+        <v>203</v>
+      </c>
+      <c r="AF16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="16"/>
+    </row>
+    <row r="17" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
         <v>12</v>
       </c>
@@ -2317,35 +2435,43 @@
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
-      <c r="I17" s="15">
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="15">
         <v>76</v>
       </c>
-      <c r="J17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
       <c r="N17" s="3"/>
       <c r="O17" s="3"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="2">
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="16"/>
+      <c r="U17" s="2">
         <v>140</v>
       </c>
-      <c r="R17" s="3"/>
-      <c r="T17" s="3"/>
-      <c r="U17" s="3"/>
       <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
       <c r="X17" s="3"/>
-      <c r="Y17" s="15">
-        <v>204</v>
-      </c>
+      <c r="Y17" s="3"/>
       <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="16"/>
-    </row>
-    <row r="18" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE17" s="15">
+        <v>204</v>
+      </c>
+      <c r="AF17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3"/>
+      <c r="AN17" s="16"/>
+    </row>
+    <row r="18" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="17">
         <v>13</v>
       </c>
@@ -2355,35 +2481,43 @@
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
-      <c r="I18" s="17">
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="17">
         <v>77</v>
       </c>
-      <c r="J18" s="3"/>
       <c r="L18" s="3"/>
-      <c r="M18" s="3"/>
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
-      <c r="P18" s="16"/>
-      <c r="Q18" s="11">
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="3"/>
+      <c r="T18" s="16"/>
+      <c r="U18" s="11">
         <v>141</v>
       </c>
-      <c r="R18" s="3"/>
-      <c r="T18" s="3"/>
-      <c r="U18" s="3"/>
       <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
       <c r="X18" s="3"/>
-      <c r="Y18" s="17">
-        <v>205</v>
-      </c>
+      <c r="Y18" s="3"/>
       <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="16"/>
-    </row>
-    <row r="19" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE18" s="17">
+        <v>205</v>
+      </c>
+      <c r="AF18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="16"/>
+    </row>
+    <row r="19" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="17">
         <v>14</v>
       </c>
@@ -2393,35 +2527,43 @@
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
-      <c r="I19" s="17">
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="17">
         <v>78</v>
       </c>
-      <c r="J19" s="3"/>
       <c r="L19" s="3"/>
-      <c r="M19" s="3"/>
       <c r="N19" s="3"/>
       <c r="O19" s="3"/>
-      <c r="P19" s="16"/>
-      <c r="Q19" s="11">
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="3"/>
+      <c r="T19" s="16"/>
+      <c r="U19" s="11">
         <v>142</v>
       </c>
-      <c r="R19" s="3"/>
-      <c r="T19" s="3"/>
-      <c r="U19" s="3"/>
       <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
       <c r="X19" s="3"/>
-      <c r="Y19" s="17">
-        <v>206</v>
-      </c>
+      <c r="Y19" s="3"/>
       <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="16"/>
-    </row>
-    <row r="20" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE19" s="17">
+        <v>206</v>
+      </c>
+      <c r="AF19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3"/>
+      <c r="AN19" s="16"/>
+    </row>
+    <row r="20" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="17">
         <v>15</v>
       </c>
@@ -2431,35 +2573,43 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
-      <c r="I20" s="17">
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="17">
         <v>79</v>
       </c>
-      <c r="J20" s="3"/>
       <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
       <c r="N20" s="3"/>
       <c r="O20" s="3"/>
-      <c r="P20" s="16"/>
-      <c r="Q20" s="11">
+      <c r="P20" s="3"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="11">
         <v>143</v>
       </c>
-      <c r="R20" s="3"/>
-      <c r="T20" s="3"/>
-      <c r="U20" s="3"/>
       <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
       <c r="X20" s="3"/>
-      <c r="Y20" s="17">
-        <v>207</v>
-      </c>
+      <c r="Y20" s="3"/>
       <c r="Z20" s="3"/>
+      <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
-      <c r="AF20" s="16"/>
-    </row>
-    <row r="21" spans="1:32" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE20" s="17">
+        <v>207</v>
+      </c>
+      <c r="AF20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3"/>
+      <c r="AK20" s="3"/>
+      <c r="AL20" s="3"/>
+      <c r="AM20" s="3"/>
+      <c r="AN20" s="16"/>
+    </row>
+    <row r="21" spans="1:40" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18">
         <v>16</v>
       </c>
@@ -2470,38 +2620,46 @@
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
-      <c r="I21" s="18">
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="18">
         <v>80</v>
       </c>
-      <c r="J21" s="8"/>
-      <c r="K21" s="7"/>
       <c r="L21" s="8"/>
-      <c r="M21" s="8"/>
+      <c r="M21" s="7"/>
       <c r="N21" s="8"/>
       <c r="O21" s="8"/>
-      <c r="P21" s="19"/>
-      <c r="Q21" s="12">
+      <c r="P21" s="8"/>
+      <c r="Q21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="12">
         <v>144</v>
       </c>
-      <c r="R21" s="8"/>
-      <c r="S21" s="7"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
       <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
+      <c r="W21" s="7"/>
       <c r="X21" s="8"/>
-      <c r="Y21" s="18">
-        <v>208</v>
-      </c>
+      <c r="Y21" s="8"/>
       <c r="Z21" s="8"/>
-      <c r="AA21" s="7"/>
+      <c r="AA21" s="8"/>
       <c r="AB21" s="8"/>
       <c r="AC21" s="8"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="5"/>
-      <c r="AF21" s="21"/>
-    </row>
-    <row r="22" spans="1:32" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="18">
+        <v>208</v>
+      </c>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="5"/>
+      <c r="AK21" s="5"/>
+      <c r="AL21" s="8"/>
+      <c r="AM21" s="8"/>
+      <c r="AN21" s="21"/>
+    </row>
+    <row r="22" spans="1:40" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <v>17</v>
       </c>
@@ -2511,35 +2669,43 @@
       <c r="F22" s="3"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
-      <c r="I22" s="15">
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="15">
         <v>81</v>
       </c>
-      <c r="J22" s="3"/>
       <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
       <c r="N22" s="3"/>
       <c r="O22" s="3"/>
-      <c r="P22" s="16"/>
-      <c r="Q22" s="2">
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="16"/>
+      <c r="U22" s="2">
         <v>145</v>
       </c>
-      <c r="R22" s="3"/>
-      <c r="T22" s="3"/>
-      <c r="U22" s="3"/>
       <c r="V22" s="3"/>
-      <c r="W22" s="3"/>
       <c r="X22" s="3"/>
-      <c r="Y22" s="15">
-        <v>209</v>
-      </c>
+      <c r="Y22" s="3"/>
       <c r="Z22" s="3"/>
+      <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
-      <c r="AD22" s="10"/>
-      <c r="AE22" s="10"/>
-      <c r="AF22" s="22"/>
-    </row>
-    <row r="23" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="15">
+        <v>209</v>
+      </c>
+      <c r="AF22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="10"/>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="3"/>
+      <c r="AM22" s="3"/>
+      <c r="AN22" s="22"/>
+    </row>
+    <row r="23" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <v>18</v>
       </c>
@@ -2549,35 +2715,43 @@
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
-      <c r="I23" s="15">
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="15">
         <v>82</v>
       </c>
-      <c r="J23" s="3"/>
       <c r="L23" s="3"/>
-      <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="16"/>
-      <c r="Q23" s="2">
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="16"/>
+      <c r="U23" s="2">
         <v>146</v>
       </c>
-      <c r="R23" s="3"/>
-      <c r="T23" s="3"/>
-      <c r="U23" s="3"/>
       <c r="V23" s="3"/>
-      <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-      <c r="Y23" s="15">
-        <v>210</v>
-      </c>
+      <c r="Y23" s="3"/>
       <c r="Z23" s="3"/>
+      <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
-      <c r="AF23" s="16"/>
-    </row>
-    <row r="24" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE23" s="15">
+        <v>210</v>
+      </c>
+      <c r="AF23" s="3"/>
+      <c r="AH23" s="3"/>
+      <c r="AI23" s="3"/>
+      <c r="AJ23" s="3"/>
+      <c r="AK23" s="3"/>
+      <c r="AL23" s="3"/>
+      <c r="AM23" s="3"/>
+      <c r="AN23" s="16"/>
+    </row>
+    <row r="24" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <v>19</v>
       </c>
@@ -2587,35 +2761,43 @@
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
-      <c r="I24" s="15">
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="15">
         <v>83</v>
       </c>
-      <c r="J24" s="3"/>
       <c r="L24" s="3"/>
-      <c r="M24" s="3"/>
       <c r="N24" s="3"/>
       <c r="O24" s="3"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="2">
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3"/>
+      <c r="T24" s="16"/>
+      <c r="U24" s="2">
         <v>147</v>
       </c>
-      <c r="R24" s="3"/>
-      <c r="T24" s="3"/>
-      <c r="U24" s="3"/>
       <c r="V24" s="3"/>
-      <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="15">
-        <v>211</v>
-      </c>
+      <c r="Y24" s="3"/>
       <c r="Z24" s="3"/>
+      <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
-      <c r="AF24" s="16"/>
-    </row>
-    <row r="25" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE24" s="15">
+        <v>211</v>
+      </c>
+      <c r="AF24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3"/>
+      <c r="AK24" s="3"/>
+      <c r="AL24" s="3"/>
+      <c r="AM24" s="3"/>
+      <c r="AN24" s="16"/>
+    </row>
+    <row r="25" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <v>20</v>
       </c>
@@ -2625,35 +2807,43 @@
       <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
-      <c r="I25" s="15">
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="15">
         <v>84</v>
       </c>
-      <c r="J25" s="3"/>
       <c r="L25" s="3"/>
-      <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="16"/>
-      <c r="Q25" s="2">
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3"/>
+      <c r="T25" s="16"/>
+      <c r="U25" s="2">
         <v>148</v>
       </c>
-      <c r="R25" s="3"/>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
       <c r="V25" s="3"/>
-      <c r="W25" s="3"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="15">
-        <v>212</v>
-      </c>
+      <c r="Y25" s="3"/>
       <c r="Z25" s="3"/>
+      <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-      <c r="AE25" s="3"/>
-      <c r="AF25" s="16"/>
-    </row>
-    <row r="26" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE25" s="15">
+        <v>212</v>
+      </c>
+      <c r="AF25" s="3"/>
+      <c r="AH25" s="3"/>
+      <c r="AI25" s="3"/>
+      <c r="AJ25" s="3"/>
+      <c r="AK25" s="3"/>
+      <c r="AL25" s="3"/>
+      <c r="AM25" s="3"/>
+      <c r="AN25" s="16"/>
+    </row>
+    <row r="26" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17">
         <v>21</v>
       </c>
@@ -2663,35 +2853,43 @@
       <c r="F26" s="3"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
-      <c r="I26" s="17">
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="17">
         <v>85</v>
       </c>
-      <c r="J26" s="3"/>
       <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="11">
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3"/>
+      <c r="T26" s="16"/>
+      <c r="U26" s="11">
         <v>149</v>
       </c>
-      <c r="R26" s="3"/>
-      <c r="T26" s="3"/>
-      <c r="U26" s="3"/>
       <c r="V26" s="3"/>
-      <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="17">
-        <v>213</v>
-      </c>
+      <c r="Y26" s="3"/>
       <c r="Z26" s="3"/>
+      <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
-      <c r="AF26" s="16"/>
-    </row>
-    <row r="27" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE26" s="17">
+        <v>213</v>
+      </c>
+      <c r="AF26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3"/>
+      <c r="AK26" s="3"/>
+      <c r="AL26" s="3"/>
+      <c r="AM26" s="3"/>
+      <c r="AN26" s="16"/>
+    </row>
+    <row r="27" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="17">
         <v>22</v>
       </c>
@@ -2701,35 +2899,43 @@
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
-      <c r="I27" s="17">
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="17">
         <v>86</v>
       </c>
-      <c r="J27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="16"/>
-      <c r="Q27" s="11">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3"/>
+      <c r="T27" s="16"/>
+      <c r="U27" s="11">
         <v>150</v>
       </c>
-      <c r="R27" s="3"/>
-      <c r="T27" s="3"/>
-      <c r="U27" s="3"/>
       <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
       <c r="X27" s="3"/>
-      <c r="Y27" s="17">
-        <v>214</v>
-      </c>
+      <c r="Y27" s="3"/>
       <c r="Z27" s="3"/>
+      <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
-      <c r="AF27" s="16"/>
-    </row>
-    <row r="28" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE27" s="17">
+        <v>214</v>
+      </c>
+      <c r="AF27" s="3"/>
+      <c r="AH27" s="3"/>
+      <c r="AI27" s="3"/>
+      <c r="AJ27" s="3"/>
+      <c r="AK27" s="3"/>
+      <c r="AL27" s="3"/>
+      <c r="AM27" s="3"/>
+      <c r="AN27" s="16"/>
+    </row>
+    <row r="28" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="17">
         <v>23</v>
       </c>
@@ -2739,35 +2945,43 @@
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
-      <c r="I28" s="17">
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="17">
         <v>87</v>
       </c>
-      <c r="J28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="16"/>
-      <c r="Q28" s="11">
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3"/>
+      <c r="T28" s="16"/>
+      <c r="U28" s="11">
         <v>151</v>
       </c>
-      <c r="R28" s="3"/>
-      <c r="T28" s="3"/>
-      <c r="U28" s="3"/>
       <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
       <c r="X28" s="3"/>
-      <c r="Y28" s="17">
-        <v>215</v>
-      </c>
+      <c r="Y28" s="3"/>
       <c r="Z28" s="3"/>
+      <c r="AA28" s="3"/>
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
-      <c r="AF28" s="16"/>
-    </row>
-    <row r="29" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE28" s="17">
+        <v>215</v>
+      </c>
+      <c r="AF28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3"/>
+      <c r="AK28" s="3"/>
+      <c r="AL28" s="3"/>
+      <c r="AM28" s="3"/>
+      <c r="AN28" s="16"/>
+    </row>
+    <row r="29" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="17">
         <v>24</v>
       </c>
@@ -2777,35 +2991,43 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="17">
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="17">
         <v>88</v>
       </c>
-      <c r="J29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="16"/>
-      <c r="Q29" s="11">
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3"/>
+      <c r="T29" s="16"/>
+      <c r="U29" s="11">
         <v>152</v>
       </c>
-      <c r="R29" s="3"/>
-      <c r="T29" s="3"/>
-      <c r="U29" s="3"/>
       <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
       <c r="X29" s="3"/>
-      <c r="Y29" s="17">
-        <v>216</v>
-      </c>
+      <c r="Y29" s="3"/>
       <c r="Z29" s="3"/>
+      <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
-      <c r="AF29" s="16"/>
-    </row>
-    <row r="30" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE29" s="17">
+        <v>216</v>
+      </c>
+      <c r="AF29" s="3"/>
+      <c r="AH29" s="3"/>
+      <c r="AI29" s="3"/>
+      <c r="AJ29" s="3"/>
+      <c r="AK29" s="3"/>
+      <c r="AL29" s="3"/>
+      <c r="AM29" s="3"/>
+      <c r="AN29" s="16"/>
+    </row>
+    <row r="30" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15">
         <v>25</v>
       </c>
@@ -2815,35 +3037,43 @@
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
-      <c r="I30" s="15">
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="15">
         <v>89</v>
       </c>
-      <c r="J30" s="3"/>
       <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="16"/>
-      <c r="Q30" s="2">
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3"/>
+      <c r="T30" s="16"/>
+      <c r="U30" s="2">
         <v>153</v>
       </c>
-      <c r="R30" s="3"/>
-      <c r="T30" s="3"/>
-      <c r="U30" s="3"/>
       <c r="V30" s="3"/>
-      <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="15">
-        <v>217</v>
-      </c>
+      <c r="Y30" s="3"/>
       <c r="Z30" s="3"/>
+      <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
-      <c r="AE30" s="3"/>
-      <c r="AF30" s="16"/>
-    </row>
-    <row r="31" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE30" s="15">
+        <v>217</v>
+      </c>
+      <c r="AF30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3"/>
+      <c r="AK30" s="3"/>
+      <c r="AL30" s="3"/>
+      <c r="AM30" s="3"/>
+      <c r="AN30" s="16"/>
+    </row>
+    <row r="31" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15">
         <v>26</v>
       </c>
@@ -2853,35 +3083,43 @@
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
-      <c r="I31" s="15">
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
+      <c r="K31" s="15">
         <v>90</v>
       </c>
-      <c r="J31" s="3"/>
       <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="16"/>
-      <c r="Q31" s="2">
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3"/>
+      <c r="T31" s="16"/>
+      <c r="U31" s="2">
         <v>154</v>
       </c>
-      <c r="R31" s="3"/>
-      <c r="T31" s="3"/>
-      <c r="U31" s="3"/>
       <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
       <c r="X31" s="3"/>
-      <c r="Y31" s="15">
-        <v>218</v>
-      </c>
+      <c r="Y31" s="3"/>
       <c r="Z31" s="3"/>
+      <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-      <c r="AE31" s="3"/>
-      <c r="AF31" s="16"/>
-    </row>
-    <row r="32" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE31" s="15">
+        <v>218</v>
+      </c>
+      <c r="AF31" s="3"/>
+      <c r="AH31" s="3"/>
+      <c r="AI31" s="3"/>
+      <c r="AJ31" s="3"/>
+      <c r="AK31" s="3"/>
+      <c r="AL31" s="3"/>
+      <c r="AM31" s="3"/>
+      <c r="AN31" s="16"/>
+    </row>
+    <row r="32" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <v>27</v>
       </c>
@@ -2891,35 +3129,43 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="15">
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="15">
         <v>91</v>
       </c>
-      <c r="J32" s="3"/>
       <c r="L32" s="3"/>
-      <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="16"/>
-      <c r="Q32" s="2">
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3"/>
+      <c r="T32" s="16"/>
+      <c r="U32" s="2">
         <v>155</v>
       </c>
-      <c r="R32" s="3"/>
-      <c r="T32" s="3"/>
-      <c r="U32" s="3"/>
       <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-      <c r="Y32" s="15">
-        <v>219</v>
-      </c>
+      <c r="Y32" s="3"/>
       <c r="Z32" s="3"/>
+      <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
-      <c r="AE32" s="3"/>
-      <c r="AF32" s="16"/>
-    </row>
-    <row r="33" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE32" s="15">
+        <v>219</v>
+      </c>
+      <c r="AF32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3"/>
+      <c r="AK32" s="3"/>
+      <c r="AL32" s="3"/>
+      <c r="AM32" s="3"/>
+      <c r="AN32" s="16"/>
+    </row>
+    <row r="33" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15">
         <v>28</v>
       </c>
@@ -2929,35 +3175,43 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="15">
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="15">
         <v>92</v>
       </c>
-      <c r="J33" s="3"/>
       <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="16"/>
-      <c r="Q33" s="2">
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="2">
         <v>156</v>
       </c>
-      <c r="R33" s="3"/>
-      <c r="T33" s="3"/>
-      <c r="U33" s="3"/>
       <c r="V33" s="3"/>
-      <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-      <c r="Y33" s="15">
-        <v>220</v>
-      </c>
+      <c r="Y33" s="3"/>
       <c r="Z33" s="3"/>
+      <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
-      <c r="AF33" s="16"/>
-    </row>
-    <row r="34" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE33" s="15">
+        <v>220</v>
+      </c>
+      <c r="AF33" s="3"/>
+      <c r="AH33" s="3"/>
+      <c r="AI33" s="3"/>
+      <c r="AJ33" s="3"/>
+      <c r="AK33" s="3"/>
+      <c r="AL33" s="3"/>
+      <c r="AM33" s="3"/>
+      <c r="AN33" s="16"/>
+    </row>
+    <row r="34" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="17">
         <v>29</v>
       </c>
@@ -2967,35 +3221,43 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="17">
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="17">
         <v>93</v>
       </c>
-      <c r="J34" s="3"/>
       <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="16"/>
-      <c r="Q34" s="11">
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="11">
         <v>157</v>
       </c>
-      <c r="R34" s="3"/>
-      <c r="T34" s="3"/>
-      <c r="U34" s="3"/>
       <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="17">
-        <v>221</v>
-      </c>
+      <c r="Y34" s="3"/>
       <c r="Z34" s="3"/>
+      <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
-      <c r="AE34" s="3"/>
-      <c r="AF34" s="16"/>
-    </row>
-    <row r="35" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE34" s="17">
+        <v>221</v>
+      </c>
+      <c r="AF34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3"/>
+      <c r="AK34" s="3"/>
+      <c r="AL34" s="3"/>
+      <c r="AM34" s="3"/>
+      <c r="AN34" s="16"/>
+    </row>
+    <row r="35" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="17">
         <v>30</v>
       </c>
@@ -3005,35 +3267,43 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="17">
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="17">
         <v>94</v>
       </c>
-      <c r="J35" s="3"/>
       <c r="L35" s="3"/>
-      <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
-      <c r="P35" s="16"/>
-      <c r="Q35" s="11">
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="11">
         <v>158</v>
       </c>
-      <c r="R35" s="3"/>
-      <c r="T35" s="3"/>
-      <c r="U35" s="3"/>
       <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="17">
-        <v>222</v>
-      </c>
+      <c r="Y35" s="3"/>
       <c r="Z35" s="3"/>
+      <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
-      <c r="AE35" s="3"/>
-      <c r="AF35" s="16"/>
-    </row>
-    <row r="36" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE35" s="17">
+        <v>222</v>
+      </c>
+      <c r="AF35" s="3"/>
+      <c r="AH35" s="3"/>
+      <c r="AI35" s="3"/>
+      <c r="AJ35" s="3"/>
+      <c r="AK35" s="3"/>
+      <c r="AL35" s="3"/>
+      <c r="AM35" s="3"/>
+      <c r="AN35" s="16"/>
+    </row>
+    <row r="36" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="17">
         <v>31</v>
       </c>
@@ -3043,35 +3313,43 @@
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
-      <c r="I36" s="17">
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="17">
         <v>95</v>
       </c>
-      <c r="J36" s="3"/>
       <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
-      <c r="P36" s="16"/>
-      <c r="Q36" s="11">
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="11">
         <v>159</v>
       </c>
-      <c r="R36" s="3"/>
-      <c r="T36" s="3"/>
-      <c r="U36" s="3"/>
       <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="17">
-        <v>223</v>
-      </c>
+      <c r="Y36" s="3"/>
       <c r="Z36" s="3"/>
+      <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
-      <c r="AE36" s="3"/>
-      <c r="AF36" s="16"/>
-    </row>
-    <row r="37" spans="1:32" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE36" s="17">
+        <v>223</v>
+      </c>
+      <c r="AF36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3"/>
+      <c r="AK36" s="3"/>
+      <c r="AL36" s="3"/>
+      <c r="AM36" s="3"/>
+      <c r="AN36" s="16"/>
+    </row>
+    <row r="37" spans="1:40" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="20">
         <v>32</v>
       </c>
@@ -3082,38 +3360,46 @@
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
       <c r="H37" s="5"/>
-      <c r="I37" s="20">
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+      <c r="K37" s="20">
         <v>96</v>
       </c>
-      <c r="J37" s="5"/>
-      <c r="K37" s="4"/>
       <c r="L37" s="5"/>
-      <c r="M37" s="5"/>
+      <c r="M37" s="4"/>
       <c r="N37" s="5"/>
       <c r="O37" s="5"/>
-      <c r="P37" s="21"/>
-      <c r="Q37" s="12">
+      <c r="P37" s="5"/>
+      <c r="Q37" s="5"/>
+      <c r="R37" s="5"/>
+      <c r="S37" s="5"/>
+      <c r="T37" s="21"/>
+      <c r="U37" s="12">
         <v>160</v>
       </c>
-      <c r="R37" s="5"/>
-      <c r="S37" s="4"/>
-      <c r="T37" s="5"/>
-      <c r="U37" s="5"/>
       <c r="V37" s="5"/>
-      <c r="W37" s="5"/>
+      <c r="W37" s="4"/>
       <c r="X37" s="5"/>
-      <c r="Y37" s="18">
-        <v>224</v>
-      </c>
+      <c r="Y37" s="5"/>
       <c r="Z37" s="5"/>
-      <c r="AA37" s="4"/>
+      <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
       <c r="AD37" s="5"/>
-      <c r="AE37" s="5"/>
-      <c r="AF37" s="21"/>
-    </row>
-    <row r="38" spans="1:32" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AE37" s="18">
+        <v>224</v>
+      </c>
+      <c r="AF37" s="5"/>
+      <c r="AG37" s="4"/>
+      <c r="AH37" s="5"/>
+      <c r="AI37" s="5"/>
+      <c r="AJ37" s="5"/>
+      <c r="AK37" s="5"/>
+      <c r="AL37" s="5"/>
+      <c r="AM37" s="5"/>
+      <c r="AN37" s="21"/>
+    </row>
+    <row r="38" spans="1:40" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13">
         <v>33</v>
       </c>
@@ -3124,38 +3410,46 @@
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="10"/>
-      <c r="I38" s="13">
+      <c r="I38" s="10"/>
+      <c r="J38" s="10"/>
+      <c r="K38" s="13">
         <v>97</v>
       </c>
-      <c r="J38" s="10"/>
-      <c r="K38" s="9"/>
       <c r="L38" s="10"/>
-      <c r="M38" s="10"/>
+      <c r="M38" s="9"/>
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
-      <c r="P38" s="22"/>
-      <c r="Q38" s="2">
+      <c r="P38" s="10"/>
+      <c r="Q38" s="10"/>
+      <c r="R38" s="10"/>
+      <c r="S38" s="10"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="2">
         <v>161</v>
       </c>
-      <c r="R38" s="10"/>
-      <c r="S38" s="9"/>
-      <c r="T38" s="10"/>
-      <c r="U38" s="10"/>
       <c r="V38" s="10"/>
-      <c r="W38" s="10"/>
+      <c r="W38" s="9"/>
       <c r="X38" s="10"/>
-      <c r="Y38" s="15">
-        <v>225</v>
-      </c>
+      <c r="Y38" s="10"/>
       <c r="Z38" s="10"/>
-      <c r="AA38" s="9"/>
+      <c r="AA38" s="10"/>
       <c r="AB38" s="10"/>
       <c r="AC38" s="10"/>
       <c r="AD38" s="10"/>
-      <c r="AE38" s="10"/>
-      <c r="AF38" s="22"/>
-    </row>
-    <row r="39" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE38" s="15">
+        <v>225</v>
+      </c>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="9"/>
+      <c r="AH38" s="10"/>
+      <c r="AI38" s="10"/>
+      <c r="AJ38" s="10"/>
+      <c r="AK38" s="10"/>
+      <c r="AL38" s="10"/>
+      <c r="AM38" s="10"/>
+      <c r="AN38" s="22"/>
+    </row>
+    <row r="39" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <v>34</v>
       </c>
@@ -3165,35 +3459,43 @@
       <c r="F39" s="3"/>
       <c r="G39" s="3"/>
       <c r="H39" s="3"/>
-      <c r="I39" s="15">
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="15">
         <v>98</v>
       </c>
-      <c r="J39" s="3"/>
       <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="16"/>
-      <c r="Q39" s="2">
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="2">
         <v>162</v>
       </c>
-      <c r="R39" s="3"/>
-      <c r="T39" s="3"/>
-      <c r="U39" s="3"/>
       <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
       <c r="X39" s="3"/>
-      <c r="Y39" s="15">
-        <v>226</v>
-      </c>
+      <c r="Y39" s="3"/>
       <c r="Z39" s="3"/>
+      <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
-      <c r="AF39" s="16"/>
-    </row>
-    <row r="40" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE39" s="15">
+        <v>226</v>
+      </c>
+      <c r="AF39" s="3"/>
+      <c r="AH39" s="3"/>
+      <c r="AI39" s="3"/>
+      <c r="AJ39" s="3"/>
+      <c r="AK39" s="3"/>
+      <c r="AL39" s="3"/>
+      <c r="AM39" s="3"/>
+      <c r="AN39" s="16"/>
+    </row>
+    <row r="40" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <v>35</v>
       </c>
@@ -3203,35 +3505,43 @@
       <c r="F40" s="3"/>
       <c r="G40" s="3"/>
       <c r="H40" s="3"/>
-      <c r="I40" s="15">
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="15">
         <v>99</v>
       </c>
-      <c r="J40" s="3"/>
       <c r="L40" s="3"/>
-      <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="16"/>
-      <c r="Q40" s="2">
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="2">
         <v>163</v>
       </c>
-      <c r="R40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="3"/>
       <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-      <c r="Y40" s="15">
-        <v>227</v>
-      </c>
+      <c r="Y40" s="3"/>
       <c r="Z40" s="3"/>
+      <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
-      <c r="AF40" s="16"/>
-    </row>
-    <row r="41" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE40" s="15">
+        <v>227</v>
+      </c>
+      <c r="AF40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3"/>
+      <c r="AL40" s="3"/>
+      <c r="AM40" s="3"/>
+      <c r="AN40" s="16"/>
+    </row>
+    <row r="41" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="15">
         <v>36</v>
       </c>
@@ -3241,35 +3551,43 @@
       <c r="F41" s="3"/>
       <c r="G41" s="3"/>
       <c r="H41" s="3"/>
-      <c r="I41" s="15">
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="15">
         <v>100</v>
       </c>
-      <c r="J41" s="3"/>
       <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="16"/>
-      <c r="Q41" s="2">
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="2">
         <v>164</v>
       </c>
-      <c r="R41" s="3"/>
-      <c r="T41" s="3"/>
-      <c r="U41" s="3"/>
       <c r="V41" s="3"/>
-      <c r="W41" s="3"/>
       <c r="X41" s="3"/>
-      <c r="Y41" s="15">
-        <v>228</v>
-      </c>
+      <c r="Y41" s="3"/>
       <c r="Z41" s="3"/>
+      <c r="AA41" s="3"/>
       <c r="AB41" s="3"/>
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
-      <c r="AE41" s="3"/>
-      <c r="AF41" s="16"/>
-    </row>
-    <row r="42" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE41" s="15">
+        <v>228</v>
+      </c>
+      <c r="AF41" s="3"/>
+      <c r="AH41" s="3"/>
+      <c r="AI41" s="3"/>
+      <c r="AJ41" s="3"/>
+      <c r="AK41" s="3"/>
+      <c r="AL41" s="3"/>
+      <c r="AM41" s="3"/>
+      <c r="AN41" s="16"/>
+    </row>
+    <row r="42" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="17">
         <v>37</v>
       </c>
@@ -3279,35 +3597,43 @@
       <c r="F42" s="3"/>
       <c r="G42" s="3"/>
       <c r="H42" s="3"/>
-      <c r="I42" s="17">
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="17">
         <v>101</v>
       </c>
-      <c r="J42" s="3"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="11">
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="11">
         <v>165</v>
       </c>
-      <c r="R42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
       <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
       <c r="X42" s="3"/>
-      <c r="Y42" s="17">
-        <v>229</v>
-      </c>
+      <c r="Y42" s="3"/>
       <c r="Z42" s="3"/>
+      <c r="AA42" s="3"/>
       <c r="AB42" s="3"/>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="16"/>
-    </row>
-    <row r="43" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE42" s="17">
+        <v>229</v>
+      </c>
+      <c r="AF42" s="3"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
+      <c r="AJ42" s="3"/>
+      <c r="AK42" s="3"/>
+      <c r="AL42" s="3"/>
+      <c r="AM42" s="3"/>
+      <c r="AN42" s="16"/>
+    </row>
+    <row r="43" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="17">
         <v>38</v>
       </c>
@@ -3317,35 +3643,43 @@
       <c r="F43" s="3"/>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="17">
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="17">
         <v>102</v>
       </c>
-      <c r="J43" s="3"/>
       <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="11">
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="11">
         <v>166</v>
       </c>
-      <c r="R43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
       <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
       <c r="X43" s="3"/>
-      <c r="Y43" s="17">
-        <v>230</v>
-      </c>
+      <c r="Y43" s="3"/>
       <c r="Z43" s="3"/>
+      <c r="AA43" s="3"/>
       <c r="AB43" s="3"/>
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
-      <c r="AE43" s="3"/>
-      <c r="AF43" s="16"/>
-    </row>
-    <row r="44" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE43" s="17">
+        <v>230</v>
+      </c>
+      <c r="AF43" s="3"/>
+      <c r="AH43" s="3"/>
+      <c r="AI43" s="3"/>
+      <c r="AJ43" s="3"/>
+      <c r="AK43" s="3"/>
+      <c r="AL43" s="3"/>
+      <c r="AM43" s="3"/>
+      <c r="AN43" s="16"/>
+    </row>
+    <row r="44" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="17">
         <v>39</v>
       </c>
@@ -3355,35 +3689,43 @@
       <c r="F44" s="3"/>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
-      <c r="I44" s="17">
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="17">
         <v>103</v>
       </c>
-      <c r="J44" s="3"/>
       <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="11">
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3"/>
+      <c r="T44" s="16"/>
+      <c r="U44" s="11">
         <v>167</v>
       </c>
-      <c r="R44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
       <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="17">
-        <v>231</v>
-      </c>
+      <c r="Y44" s="3"/>
       <c r="Z44" s="3"/>
+      <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
-      <c r="AE44" s="3"/>
-      <c r="AF44" s="16"/>
-    </row>
-    <row r="45" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE44" s="17">
+        <v>231</v>
+      </c>
+      <c r="AF44" s="3"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
+      <c r="AJ44" s="3"/>
+      <c r="AK44" s="3"/>
+      <c r="AL44" s="3"/>
+      <c r="AM44" s="3"/>
+      <c r="AN44" s="16"/>
+    </row>
+    <row r="45" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="17">
         <v>40</v>
       </c>
@@ -3393,35 +3735,43 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
-      <c r="I45" s="17">
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="17">
         <v>104</v>
       </c>
-      <c r="J45" s="3"/>
       <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
-      <c r="P45" s="16"/>
-      <c r="Q45" s="11">
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3"/>
+      <c r="T45" s="16"/>
+      <c r="U45" s="11">
         <v>168</v>
       </c>
-      <c r="R45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
       <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
       <c r="X45" s="3"/>
-      <c r="Y45" s="17">
-        <v>232</v>
-      </c>
+      <c r="Y45" s="3"/>
       <c r="Z45" s="3"/>
+      <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
-      <c r="AE45" s="3"/>
-      <c r="AF45" s="16"/>
-    </row>
-    <row r="46" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE45" s="17">
+        <v>232</v>
+      </c>
+      <c r="AF45" s="3"/>
+      <c r="AH45" s="3"/>
+      <c r="AI45" s="3"/>
+      <c r="AJ45" s="3"/>
+      <c r="AK45" s="3"/>
+      <c r="AL45" s="3"/>
+      <c r="AM45" s="3"/>
+      <c r="AN45" s="16"/>
+    </row>
+    <row r="46" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="15">
         <v>41</v>
       </c>
@@ -3431,35 +3781,43 @@
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
       <c r="H46" s="3"/>
-      <c r="I46" s="15">
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="15">
         <v>105</v>
       </c>
-      <c r="J46" s="3"/>
       <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="16"/>
-      <c r="Q46" s="2">
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3"/>
+      <c r="T46" s="16"/>
+      <c r="U46" s="2">
         <v>169</v>
       </c>
-      <c r="R46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
       <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
       <c r="X46" s="3"/>
-      <c r="Y46" s="15">
-        <v>233</v>
-      </c>
+      <c r="Y46" s="3"/>
       <c r="Z46" s="3"/>
+      <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
-      <c r="AE46" s="3"/>
-      <c r="AF46" s="16"/>
-    </row>
-    <row r="47" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE46" s="15">
+        <v>233</v>
+      </c>
+      <c r="AF46" s="3"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="3"/>
+      <c r="AJ46" s="3"/>
+      <c r="AK46" s="3"/>
+      <c r="AL46" s="3"/>
+      <c r="AM46" s="3"/>
+      <c r="AN46" s="16"/>
+    </row>
+    <row r="47" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <v>42</v>
       </c>
@@ -3469,35 +3827,43 @@
       <c r="F47" s="3"/>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
-      <c r="I47" s="15">
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="15">
         <v>106</v>
       </c>
-      <c r="J47" s="3"/>
       <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
       <c r="N47" s="3"/>
       <c r="O47" s="3"/>
-      <c r="P47" s="16"/>
-      <c r="Q47" s="2">
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="2">
         <v>170</v>
       </c>
-      <c r="R47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
       <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
       <c r="X47" s="3"/>
-      <c r="Y47" s="15">
-        <v>234</v>
-      </c>
+      <c r="Y47" s="3"/>
       <c r="Z47" s="3"/>
+      <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
-      <c r="AE47" s="3"/>
-      <c r="AF47" s="16"/>
-    </row>
-    <row r="48" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE47" s="15">
+        <v>234</v>
+      </c>
+      <c r="AF47" s="3"/>
+      <c r="AH47" s="3"/>
+      <c r="AI47" s="3"/>
+      <c r="AJ47" s="3"/>
+      <c r="AK47" s="3"/>
+      <c r="AL47" s="3"/>
+      <c r="AM47" s="3"/>
+      <c r="AN47" s="16"/>
+    </row>
+    <row r="48" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <v>43</v>
       </c>
@@ -3507,35 +3873,43 @@
       <c r="F48" s="3"/>
       <c r="G48" s="3"/>
       <c r="H48" s="3"/>
-      <c r="I48" s="15">
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="15">
         <v>107</v>
       </c>
-      <c r="J48" s="3"/>
       <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="3"/>
-      <c r="P48" s="16"/>
-      <c r="Q48" s="2">
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3"/>
+      <c r="T48" s="16"/>
+      <c r="U48" s="2">
         <v>171</v>
       </c>
-      <c r="R48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
       <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-      <c r="Y48" s="15">
-        <v>235</v>
-      </c>
+      <c r="Y48" s="3"/>
       <c r="Z48" s="3"/>
+      <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
-      <c r="AE48" s="3"/>
-      <c r="AF48" s="16"/>
-    </row>
-    <row r="49" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE48" s="15">
+        <v>235</v>
+      </c>
+      <c r="AF48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3"/>
+      <c r="AK48" s="3"/>
+      <c r="AL48" s="3"/>
+      <c r="AM48" s="3"/>
+      <c r="AN48" s="16"/>
+    </row>
+    <row r="49" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <v>44</v>
       </c>
@@ -3545,35 +3919,43 @@
       <c r="F49" s="3"/>
       <c r="G49" s="3"/>
       <c r="H49" s="3"/>
-      <c r="I49" s="15">
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="15">
         <v>108</v>
       </c>
-      <c r="J49" s="3"/>
       <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
       <c r="N49" s="3"/>
       <c r="O49" s="3"/>
-      <c r="P49" s="16"/>
-      <c r="Q49" s="2">
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="16"/>
+      <c r="U49" s="2">
         <v>172</v>
       </c>
-      <c r="R49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
       <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
       <c r="X49" s="3"/>
-      <c r="Y49" s="15">
-        <v>236</v>
-      </c>
+      <c r="Y49" s="3"/>
       <c r="Z49" s="3"/>
+      <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
-      <c r="AE49" s="3"/>
-      <c r="AF49" s="16"/>
-    </row>
-    <row r="50" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE49" s="15">
+        <v>236</v>
+      </c>
+      <c r="AF49" s="3"/>
+      <c r="AH49" s="3"/>
+      <c r="AI49" s="3"/>
+      <c r="AJ49" s="3"/>
+      <c r="AK49" s="3"/>
+      <c r="AL49" s="3"/>
+      <c r="AM49" s="3"/>
+      <c r="AN49" s="16"/>
+    </row>
+    <row r="50" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="17">
         <v>45</v>
       </c>
@@ -3583,35 +3965,43 @@
       <c r="F50" s="3"/>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
-      <c r="I50" s="17">
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="17">
         <v>109</v>
       </c>
-      <c r="J50" s="3"/>
       <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
-      <c r="P50" s="16"/>
-      <c r="Q50" s="11">
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="16"/>
+      <c r="U50" s="11">
         <v>173</v>
       </c>
-      <c r="R50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
       <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="Y50" s="17">
-        <v>237</v>
-      </c>
+      <c r="Y50" s="3"/>
       <c r="Z50" s="3"/>
+      <c r="AA50" s="3"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
-      <c r="AE50" s="3"/>
-      <c r="AF50" s="16"/>
-    </row>
-    <row r="51" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE50" s="17">
+        <v>237</v>
+      </c>
+      <c r="AF50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3"/>
+      <c r="AL50" s="3"/>
+      <c r="AM50" s="3"/>
+      <c r="AN50" s="16"/>
+    </row>
+    <row r="51" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="17">
         <v>46</v>
       </c>
@@ -3621,35 +4011,43 @@
       <c r="F51" s="3"/>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
-      <c r="I51" s="17">
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="17">
         <v>110</v>
       </c>
-      <c r="J51" s="3"/>
       <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
-      <c r="P51" s="16"/>
-      <c r="Q51" s="11">
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="11">
         <v>174</v>
       </c>
-      <c r="R51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
       <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
       <c r="X51" s="3"/>
-      <c r="Y51" s="17">
-        <v>238</v>
-      </c>
+      <c r="Y51" s="3"/>
       <c r="Z51" s="3"/>
+      <c r="AA51" s="3"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
-      <c r="AE51" s="3"/>
-      <c r="AF51" s="16"/>
-    </row>
-    <row r="52" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE51" s="17">
+        <v>238</v>
+      </c>
+      <c r="AF51" s="3"/>
+      <c r="AH51" s="3"/>
+      <c r="AI51" s="3"/>
+      <c r="AJ51" s="3"/>
+      <c r="AK51" s="3"/>
+      <c r="AL51" s="3"/>
+      <c r="AM51" s="3"/>
+      <c r="AN51" s="16"/>
+    </row>
+    <row r="52" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="17">
         <v>47</v>
       </c>
@@ -3659,35 +4057,43 @@
       <c r="F52" s="3"/>
       <c r="G52" s="3"/>
       <c r="H52" s="3"/>
-      <c r="I52" s="17">
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="17">
         <v>111</v>
       </c>
-      <c r="J52" s="3"/>
       <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
       <c r="N52" s="3"/>
       <c r="O52" s="3"/>
-      <c r="P52" s="16"/>
-      <c r="Q52" s="11">
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3"/>
+      <c r="T52" s="16"/>
+      <c r="U52" s="11">
         <v>175</v>
       </c>
-      <c r="R52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
       <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
       <c r="X52" s="3"/>
-      <c r="Y52" s="17">
-        <v>239</v>
-      </c>
+      <c r="Y52" s="3"/>
       <c r="Z52" s="3"/>
+      <c r="AA52" s="3"/>
       <c r="AB52" s="3"/>
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
-      <c r="AE52" s="3"/>
-      <c r="AF52" s="16"/>
-    </row>
-    <row r="53" spans="1:32" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE52" s="17">
+        <v>239</v>
+      </c>
+      <c r="AF52" s="3"/>
+      <c r="AH52" s="3"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="3"/>
+      <c r="AK52" s="3"/>
+      <c r="AL52" s="3"/>
+      <c r="AM52" s="3"/>
+      <c r="AN52" s="16"/>
+    </row>
+    <row r="53" spans="1:40" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="20">
         <v>48</v>
       </c>
@@ -3698,38 +4104,46 @@
       <c r="F53" s="5"/>
       <c r="G53" s="5"/>
       <c r="H53" s="5"/>
-      <c r="I53" s="20">
+      <c r="I53" s="5"/>
+      <c r="J53" s="5"/>
+      <c r="K53" s="20">
         <v>112</v>
       </c>
-      <c r="J53" s="5"/>
-      <c r="K53" s="4"/>
       <c r="L53" s="5"/>
-      <c r="M53" s="5"/>
+      <c r="M53" s="4"/>
       <c r="N53" s="5"/>
       <c r="O53" s="5"/>
-      <c r="P53" s="21"/>
-      <c r="Q53" s="12">
+      <c r="P53" s="5"/>
+      <c r="Q53" s="5"/>
+      <c r="R53" s="5"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="21"/>
+      <c r="U53" s="12">
         <v>176</v>
       </c>
-      <c r="R53" s="5"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="5"/>
-      <c r="U53" s="5"/>
       <c r="V53" s="5"/>
-      <c r="W53" s="5"/>
+      <c r="W53" s="4"/>
       <c r="X53" s="5"/>
-      <c r="Y53" s="18">
-        <v>240</v>
-      </c>
+      <c r="Y53" s="5"/>
       <c r="Z53" s="5"/>
-      <c r="AA53" s="4"/>
+      <c r="AA53" s="5"/>
       <c r="AB53" s="5"/>
       <c r="AC53" s="5"/>
       <c r="AD53" s="5"/>
-      <c r="AE53" s="5"/>
-      <c r="AF53" s="21"/>
-    </row>
-    <row r="54" spans="1:32" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="AE53" s="18">
+        <v>240</v>
+      </c>
+      <c r="AF53" s="5"/>
+      <c r="AG53" s="4"/>
+      <c r="AH53" s="5"/>
+      <c r="AI53" s="5"/>
+      <c r="AJ53" s="5"/>
+      <c r="AK53" s="5"/>
+      <c r="AL53" s="5"/>
+      <c r="AM53" s="5"/>
+      <c r="AN53" s="21"/>
+    </row>
+    <row r="54" spans="1:40" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A54" s="13">
         <v>49</v>
       </c>
@@ -3740,38 +4154,46 @@
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
-      <c r="I54" s="13">
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="13">
         <v>113</v>
       </c>
-      <c r="J54" s="10"/>
-      <c r="K54" s="9"/>
       <c r="L54" s="10"/>
-      <c r="M54" s="10"/>
+      <c r="M54" s="9"/>
       <c r="N54" s="10"/>
       <c r="O54" s="10"/>
-      <c r="P54" s="22"/>
-      <c r="Q54" s="2">
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="22"/>
+      <c r="U54" s="2">
         <v>177</v>
       </c>
-      <c r="R54" s="10"/>
-      <c r="S54" s="9"/>
-      <c r="T54" s="10"/>
-      <c r="U54" s="10"/>
       <c r="V54" s="10"/>
-      <c r="W54" s="10"/>
+      <c r="W54" s="9"/>
       <c r="X54" s="10"/>
-      <c r="Y54" s="15">
-        <v>241</v>
-      </c>
+      <c r="Y54" s="10"/>
       <c r="Z54" s="10"/>
-      <c r="AA54" s="9"/>
+      <c r="AA54" s="10"/>
       <c r="AB54" s="10"/>
       <c r="AC54" s="10"/>
       <c r="AD54" s="10"/>
-      <c r="AE54" s="10"/>
-      <c r="AF54" s="22"/>
-    </row>
-    <row r="55" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE54" s="15">
+        <v>241</v>
+      </c>
+      <c r="AF54" s="10"/>
+      <c r="AG54" s="9"/>
+      <c r="AH54" s="10"/>
+      <c r="AI54" s="10"/>
+      <c r="AJ54" s="10"/>
+      <c r="AK54" s="10"/>
+      <c r="AL54" s="10"/>
+      <c r="AM54" s="10"/>
+      <c r="AN54" s="22"/>
+    </row>
+    <row r="55" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <v>50</v>
       </c>
@@ -3781,35 +4203,43 @@
       <c r="F55" s="3"/>
       <c r="G55" s="3"/>
       <c r="H55" s="3"/>
-      <c r="I55" s="15">
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="15">
         <v>114</v>
       </c>
-      <c r="J55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
       <c r="N55" s="3"/>
       <c r="O55" s="3"/>
-      <c r="P55" s="16"/>
-      <c r="Q55" s="2">
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3"/>
+      <c r="T55" s="16"/>
+      <c r="U55" s="2">
         <v>178</v>
       </c>
-      <c r="R55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
       <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
       <c r="X55" s="3"/>
-      <c r="Y55" s="15">
-        <v>242</v>
-      </c>
+      <c r="Y55" s="3"/>
       <c r="Z55" s="3"/>
+      <c r="AA55" s="3"/>
       <c r="AB55" s="3"/>
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
-      <c r="AE55" s="3"/>
-      <c r="AF55" s="16"/>
-    </row>
-    <row r="56" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE55" s="15">
+        <v>242</v>
+      </c>
+      <c r="AF55" s="3"/>
+      <c r="AH55" s="3"/>
+      <c r="AI55" s="3"/>
+      <c r="AJ55" s="3"/>
+      <c r="AK55" s="3"/>
+      <c r="AL55" s="3"/>
+      <c r="AM55" s="3"/>
+      <c r="AN55" s="16"/>
+    </row>
+    <row r="56" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <v>51</v>
       </c>
@@ -3819,35 +4249,43 @@
       <c r="F56" s="3"/>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
-      <c r="I56" s="15">
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="15">
         <v>115</v>
       </c>
-      <c r="J56" s="3"/>
       <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
       <c r="N56" s="3"/>
       <c r="O56" s="3"/>
-      <c r="P56" s="16"/>
-      <c r="Q56" s="2">
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3"/>
+      <c r="T56" s="16"/>
+      <c r="U56" s="2">
         <v>179</v>
       </c>
-      <c r="R56" s="3"/>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
       <c r="V56" s="3"/>
-      <c r="W56" s="3"/>
       <c r="X56" s="3"/>
-      <c r="Y56" s="15">
-        <v>243</v>
-      </c>
+      <c r="Y56" s="3"/>
       <c r="Z56" s="3"/>
+      <c r="AA56" s="3"/>
       <c r="AB56" s="3"/>
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
-      <c r="AE56" s="3"/>
-      <c r="AF56" s="16"/>
-    </row>
-    <row r="57" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE56" s="15">
+        <v>243</v>
+      </c>
+      <c r="AF56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3"/>
+      <c r="AK56" s="3"/>
+      <c r="AL56" s="3"/>
+      <c r="AM56" s="3"/>
+      <c r="AN56" s="16"/>
+    </row>
+    <row r="57" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="15">
         <v>52</v>
       </c>
@@ -3857,35 +4295,43 @@
       <c r="F57" s="3"/>
       <c r="G57" s="3"/>
       <c r="H57" s="3"/>
-      <c r="I57" s="15">
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="15">
         <v>116</v>
       </c>
-      <c r="J57" s="3"/>
       <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
       <c r="N57" s="3"/>
       <c r="O57" s="3"/>
-      <c r="P57" s="16"/>
-      <c r="Q57" s="2">
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3"/>
+      <c r="T57" s="16"/>
+      <c r="U57" s="2">
         <v>180</v>
       </c>
-      <c r="R57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
       <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
       <c r="X57" s="3"/>
-      <c r="Y57" s="15">
-        <v>244</v>
-      </c>
+      <c r="Y57" s="3"/>
       <c r="Z57" s="3"/>
+      <c r="AA57" s="3"/>
       <c r="AB57" s="3"/>
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
-      <c r="AE57" s="3"/>
-      <c r="AF57" s="16"/>
-    </row>
-    <row r="58" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE57" s="15">
+        <v>244</v>
+      </c>
+      <c r="AF57" s="3"/>
+      <c r="AH57" s="3"/>
+      <c r="AI57" s="3"/>
+      <c r="AJ57" s="3"/>
+      <c r="AK57" s="3"/>
+      <c r="AL57" s="3"/>
+      <c r="AM57" s="3"/>
+      <c r="AN57" s="16"/>
+    </row>
+    <row r="58" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="17">
         <v>53</v>
       </c>
@@ -3895,35 +4341,43 @@
       <c r="F58" s="3"/>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
-      <c r="I58" s="17">
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="17">
         <v>117</v>
       </c>
-      <c r="J58" s="3"/>
       <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
       <c r="N58" s="3"/>
       <c r="O58" s="3"/>
-      <c r="P58" s="16"/>
-      <c r="Q58" s="11">
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3"/>
+      <c r="T58" s="16"/>
+      <c r="U58" s="11">
         <v>181</v>
       </c>
-      <c r="R58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
       <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
       <c r="X58" s="3"/>
-      <c r="Y58" s="17">
-        <v>245</v>
-      </c>
+      <c r="Y58" s="3"/>
       <c r="Z58" s="3"/>
+      <c r="AA58" s="3"/>
       <c r="AB58" s="3"/>
       <c r="AC58" s="3"/>
       <c r="AD58" s="3"/>
-      <c r="AE58" s="3"/>
-      <c r="AF58" s="16"/>
-    </row>
-    <row r="59" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE58" s="17">
+        <v>245</v>
+      </c>
+      <c r="AF58" s="3"/>
+      <c r="AH58" s="3"/>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="3"/>
+      <c r="AK58" s="3"/>
+      <c r="AL58" s="3"/>
+      <c r="AM58" s="3"/>
+      <c r="AN58" s="16"/>
+    </row>
+    <row r="59" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="17">
         <v>54</v>
       </c>
@@ -3933,35 +4387,43 @@
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
-      <c r="I59" s="17">
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="17">
         <v>118</v>
       </c>
-      <c r="J59" s="3"/>
       <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="3"/>
-      <c r="P59" s="16"/>
-      <c r="Q59" s="11">
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3"/>
+      <c r="T59" s="16"/>
+      <c r="U59" s="11">
         <v>182</v>
       </c>
-      <c r="R59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
       <c r="V59" s="3"/>
-      <c r="W59" s="3"/>
       <c r="X59" s="3"/>
-      <c r="Y59" s="17">
-        <v>246</v>
-      </c>
+      <c r="Y59" s="3"/>
       <c r="Z59" s="3"/>
+      <c r="AA59" s="3"/>
       <c r="AB59" s="3"/>
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
-      <c r="AE59" s="3"/>
-      <c r="AF59" s="16"/>
-    </row>
-    <row r="60" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE59" s="17">
+        <v>246</v>
+      </c>
+      <c r="AF59" s="3"/>
+      <c r="AH59" s="3"/>
+      <c r="AI59" s="3"/>
+      <c r="AJ59" s="3"/>
+      <c r="AK59" s="3"/>
+      <c r="AL59" s="3"/>
+      <c r="AM59" s="3"/>
+      <c r="AN59" s="16"/>
+    </row>
+    <row r="60" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="17">
         <v>55</v>
       </c>
@@ -3971,35 +4433,43 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="3"/>
-      <c r="I60" s="17">
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="17">
         <v>119</v>
       </c>
-      <c r="J60" s="3"/>
       <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="3"/>
-      <c r="P60" s="16"/>
-      <c r="Q60" s="11">
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+      <c r="S60" s="3"/>
+      <c r="T60" s="16"/>
+      <c r="U60" s="11">
         <v>183</v>
       </c>
-      <c r="R60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
       <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
       <c r="X60" s="3"/>
-      <c r="Y60" s="17">
-        <v>247</v>
-      </c>
+      <c r="Y60" s="3"/>
       <c r="Z60" s="3"/>
+      <c r="AA60" s="3"/>
       <c r="AB60" s="3"/>
       <c r="AC60" s="3"/>
       <c r="AD60" s="3"/>
-      <c r="AE60" s="3"/>
-      <c r="AF60" s="16"/>
-    </row>
-    <row r="61" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE60" s="17">
+        <v>247</v>
+      </c>
+      <c r="AF60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3"/>
+      <c r="AK60" s="3"/>
+      <c r="AL60" s="3"/>
+      <c r="AM60" s="3"/>
+      <c r="AN60" s="16"/>
+    </row>
+    <row r="61" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="17">
         <v>56</v>
       </c>
@@ -4009,35 +4479,43 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="3"/>
-      <c r="I61" s="17">
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="17">
         <v>120</v>
       </c>
-      <c r="J61" s="3"/>
       <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="3"/>
-      <c r="P61" s="16"/>
-      <c r="Q61" s="11">
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+      <c r="S61" s="3"/>
+      <c r="T61" s="16"/>
+      <c r="U61" s="11">
         <v>184</v>
       </c>
-      <c r="R61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
       <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
       <c r="X61" s="3"/>
-      <c r="Y61" s="17">
-        <v>248</v>
-      </c>
+      <c r="Y61" s="3"/>
       <c r="Z61" s="3"/>
+      <c r="AA61" s="3"/>
       <c r="AB61" s="3"/>
       <c r="AC61" s="3"/>
       <c r="AD61" s="3"/>
-      <c r="AE61" s="3"/>
-      <c r="AF61" s="16"/>
-    </row>
-    <row r="62" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE61" s="17">
+        <v>248</v>
+      </c>
+      <c r="AF61" s="3"/>
+      <c r="AH61" s="3"/>
+      <c r="AI61" s="3"/>
+      <c r="AJ61" s="3"/>
+      <c r="AK61" s="3"/>
+      <c r="AL61" s="3"/>
+      <c r="AM61" s="3"/>
+      <c r="AN61" s="16"/>
+    </row>
+    <row r="62" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="15">
         <v>57</v>
       </c>
@@ -4047,35 +4525,43 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="3"/>
-      <c r="I62" s="15">
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="15">
         <v>121</v>
       </c>
-      <c r="J62" s="3"/>
       <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="3"/>
-      <c r="P62" s="16"/>
-      <c r="Q62" s="2">
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+      <c r="S62" s="3"/>
+      <c r="T62" s="16"/>
+      <c r="U62" s="2">
         <v>185</v>
       </c>
-      <c r="R62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
       <c r="V62" s="3"/>
-      <c r="W62" s="3"/>
       <c r="X62" s="3"/>
-      <c r="Y62" s="15">
-        <v>249</v>
-      </c>
+      <c r="Y62" s="3"/>
       <c r="Z62" s="3"/>
+      <c r="AA62" s="3"/>
       <c r="AB62" s="3"/>
       <c r="AC62" s="3"/>
       <c r="AD62" s="3"/>
-      <c r="AE62" s="3"/>
-      <c r="AF62" s="16"/>
-    </row>
-    <row r="63" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE62" s="15">
+        <v>249</v>
+      </c>
+      <c r="AF62" s="3"/>
+      <c r="AH62" s="3"/>
+      <c r="AI62" s="3"/>
+      <c r="AJ62" s="3"/>
+      <c r="AK62" s="3"/>
+      <c r="AL62" s="3"/>
+      <c r="AM62" s="3"/>
+      <c r="AN62" s="16"/>
+    </row>
+    <row r="63" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <v>58</v>
       </c>
@@ -4085,35 +4571,43 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
-      <c r="I63" s="15">
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="15">
         <v>122</v>
       </c>
-      <c r="J63" s="3"/>
       <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
       <c r="N63" s="3"/>
       <c r="O63" s="3"/>
-      <c r="P63" s="16"/>
-      <c r="Q63" s="2">
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
+      <c r="S63" s="3"/>
+      <c r="T63" s="16"/>
+      <c r="U63" s="2">
         <v>186</v>
       </c>
-      <c r="R63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
       <c r="V63" s="3"/>
-      <c r="W63" s="3"/>
       <c r="X63" s="3"/>
-      <c r="Y63" s="15">
-        <v>250</v>
-      </c>
+      <c r="Y63" s="3"/>
       <c r="Z63" s="3"/>
+      <c r="AA63" s="3"/>
       <c r="AB63" s="3"/>
       <c r="AC63" s="3"/>
       <c r="AD63" s="3"/>
-      <c r="AE63" s="3"/>
-      <c r="AF63" s="16"/>
-    </row>
-    <row r="64" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE63" s="15">
+        <v>250</v>
+      </c>
+      <c r="AF63" s="3"/>
+      <c r="AH63" s="3"/>
+      <c r="AI63" s="3"/>
+      <c r="AJ63" s="3"/>
+      <c r="AK63" s="3"/>
+      <c r="AL63" s="3"/>
+      <c r="AM63" s="3"/>
+      <c r="AN63" s="16"/>
+    </row>
+    <row r="64" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="15">
         <v>59</v>
       </c>
@@ -4123,35 +4617,43 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
-      <c r="I64" s="15">
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="15">
         <v>123</v>
       </c>
-      <c r="J64" s="3"/>
       <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="3"/>
-      <c r="P64" s="16"/>
-      <c r="Q64" s="2">
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3"/>
+      <c r="T64" s="16"/>
+      <c r="U64" s="2">
         <v>187</v>
       </c>
-      <c r="R64" s="3"/>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
       <c r="V64" s="3"/>
-      <c r="W64" s="3"/>
       <c r="X64" s="3"/>
-      <c r="Y64" s="15">
-        <v>251</v>
-      </c>
+      <c r="Y64" s="3"/>
       <c r="Z64" s="3"/>
+      <c r="AA64" s="3"/>
       <c r="AB64" s="3"/>
       <c r="AC64" s="3"/>
       <c r="AD64" s="3"/>
-      <c r="AE64" s="3"/>
-      <c r="AF64" s="16"/>
-    </row>
-    <row r="65" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE64" s="15">
+        <v>251</v>
+      </c>
+      <c r="AF64" s="3"/>
+      <c r="AH64" s="3"/>
+      <c r="AI64" s="3"/>
+      <c r="AJ64" s="3"/>
+      <c r="AK64" s="3"/>
+      <c r="AL64" s="3"/>
+      <c r="AM64" s="3"/>
+      <c r="AN64" s="16"/>
+    </row>
+    <row r="65" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="15">
         <v>60</v>
       </c>
@@ -4161,35 +4663,43 @@
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
-      <c r="I65" s="15">
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="15">
         <v>124</v>
       </c>
-      <c r="J65" s="3"/>
       <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
       <c r="N65" s="3"/>
       <c r="O65" s="3"/>
-      <c r="P65" s="16"/>
-      <c r="Q65" s="2">
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
+      <c r="S65" s="3"/>
+      <c r="T65" s="16"/>
+      <c r="U65" s="2">
         <v>188</v>
       </c>
-      <c r="R65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
       <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
       <c r="X65" s="3"/>
-      <c r="Y65" s="15">
-        <v>252</v>
-      </c>
+      <c r="Y65" s="3"/>
       <c r="Z65" s="3"/>
+      <c r="AA65" s="3"/>
       <c r="AB65" s="3"/>
       <c r="AC65" s="3"/>
       <c r="AD65" s="3"/>
-      <c r="AE65" s="3"/>
-      <c r="AF65" s="16"/>
-    </row>
-    <row r="66" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE65" s="15">
+        <v>252</v>
+      </c>
+      <c r="AF65" s="3"/>
+      <c r="AH65" s="3"/>
+      <c r="AI65" s="3"/>
+      <c r="AJ65" s="3"/>
+      <c r="AK65" s="3"/>
+      <c r="AL65" s="3"/>
+      <c r="AM65" s="3"/>
+      <c r="AN65" s="16"/>
+    </row>
+    <row r="66" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="17">
         <v>61</v>
       </c>
@@ -4199,35 +4709,43 @@
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
-      <c r="I66" s="17">
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="17">
         <v>125</v>
       </c>
-      <c r="J66" s="3"/>
       <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
       <c r="N66" s="3"/>
       <c r="O66" s="3"/>
-      <c r="P66" s="16"/>
-      <c r="Q66" s="11">
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+      <c r="S66" s="3"/>
+      <c r="T66" s="16"/>
+      <c r="U66" s="11">
         <v>189</v>
       </c>
-      <c r="R66" s="3"/>
-      <c r="T66" s="3"/>
-      <c r="U66" s="3"/>
       <c r="V66" s="3"/>
-      <c r="W66" s="3"/>
       <c r="X66" s="3"/>
-      <c r="Y66" s="17">
-        <v>253</v>
-      </c>
+      <c r="Y66" s="3"/>
       <c r="Z66" s="3"/>
+      <c r="AA66" s="3"/>
       <c r="AB66" s="3"/>
       <c r="AC66" s="3"/>
       <c r="AD66" s="3"/>
-      <c r="AE66" s="3"/>
-      <c r="AF66" s="16"/>
-    </row>
-    <row r="67" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE66" s="17">
+        <v>253</v>
+      </c>
+      <c r="AF66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3"/>
+      <c r="AK66" s="3"/>
+      <c r="AL66" s="3"/>
+      <c r="AM66" s="3"/>
+      <c r="AN66" s="16"/>
+    </row>
+    <row r="67" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="17">
         <v>62</v>
       </c>
@@ -4237,35 +4755,43 @@
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="3"/>
-      <c r="I67" s="17">
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="17">
         <v>126</v>
       </c>
-      <c r="J67" s="3"/>
       <c r="L67" s="3"/>
-      <c r="M67" s="3"/>
       <c r="N67" s="3"/>
       <c r="O67" s="3"/>
-      <c r="P67" s="16"/>
-      <c r="Q67" s="11">
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
+      <c r="S67" s="3"/>
+      <c r="T67" s="16"/>
+      <c r="U67" s="11">
         <v>190</v>
       </c>
-      <c r="R67" s="3"/>
-      <c r="T67" s="3"/>
-      <c r="U67" s="3"/>
       <c r="V67" s="3"/>
-      <c r="W67" s="3"/>
       <c r="X67" s="3"/>
-      <c r="Y67" s="17">
-        <v>254</v>
-      </c>
+      <c r="Y67" s="3"/>
       <c r="Z67" s="3"/>
+      <c r="AA67" s="3"/>
       <c r="AB67" s="3"/>
       <c r="AC67" s="3"/>
       <c r="AD67" s="3"/>
-      <c r="AE67" s="3"/>
-      <c r="AF67" s="16"/>
-    </row>
-    <row r="68" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AE67" s="17">
+        <v>254</v>
+      </c>
+      <c r="AF67" s="3"/>
+      <c r="AH67" s="3"/>
+      <c r="AI67" s="3"/>
+      <c r="AJ67" s="3"/>
+      <c r="AK67" s="3"/>
+      <c r="AL67" s="3"/>
+      <c r="AM67" s="3"/>
+      <c r="AN67" s="16"/>
+    </row>
+    <row r="68" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="17">
         <v>63</v>
       </c>
@@ -4275,35 +4801,43 @@
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>
-      <c r="I68" s="17">
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="17">
         <v>127</v>
       </c>
-      <c r="J68" s="3"/>
       <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
-      <c r="P68" s="16"/>
-      <c r="Q68" s="11">
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
+      <c r="S68" s="3"/>
+      <c r="T68" s="16"/>
+      <c r="U68" s="11">
         <v>191</v>
       </c>
-      <c r="R68" s="3"/>
-      <c r="T68" s="3"/>
-      <c r="U68" s="3"/>
       <c r="V68" s="3"/>
-      <c r="W68" s="3"/>
       <c r="X68" s="3"/>
-      <c r="Y68" s="17">
-        <v>255</v>
-      </c>
+      <c r="Y68" s="3"/>
       <c r="Z68" s="3"/>
+      <c r="AA68" s="3"/>
       <c r="AB68" s="3"/>
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
-      <c r="AE68" s="3"/>
-      <c r="AF68" s="16"/>
-    </row>
-    <row r="69" spans="1:32" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE68" s="17">
+        <v>255</v>
+      </c>
+      <c r="AF68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3"/>
+      <c r="AL68" s="3"/>
+      <c r="AM68" s="3"/>
+      <c r="AN68" s="16"/>
+    </row>
+    <row r="69" spans="1:40" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="18">
         <v>64</v>
       </c>
@@ -4314,48 +4848,56 @@
       <c r="F69" s="8"/>
       <c r="G69" s="8"/>
       <c r="H69" s="8"/>
-      <c r="I69" s="18">
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="18">
         <v>128</v>
       </c>
-      <c r="J69" s="8"/>
-      <c r="K69" s="7"/>
       <c r="L69" s="8"/>
-      <c r="M69" s="8"/>
+      <c r="M69" s="7"/>
       <c r="N69" s="8"/>
       <c r="O69" s="8"/>
-      <c r="P69" s="19"/>
-      <c r="Q69" s="12">
+      <c r="P69" s="8"/>
+      <c r="Q69" s="8"/>
+      <c r="R69" s="8"/>
+      <c r="S69" s="8"/>
+      <c r="T69" s="19"/>
+      <c r="U69" s="12">
         <v>192</v>
       </c>
-      <c r="R69" s="8"/>
-      <c r="S69" s="7"/>
-      <c r="T69" s="8"/>
-      <c r="U69" s="8"/>
       <c r="V69" s="8"/>
-      <c r="W69" s="8"/>
+      <c r="W69" s="7"/>
       <c r="X69" s="8"/>
-      <c r="Y69" s="18">
-        <v>256</v>
-      </c>
+      <c r="Y69" s="8"/>
       <c r="Z69" s="8"/>
-      <c r="AA69" s="7"/>
+      <c r="AA69" s="8"/>
       <c r="AB69" s="8"/>
       <c r="AC69" s="8"/>
       <c r="AD69" s="8"/>
-      <c r="AE69" s="8"/>
-      <c r="AF69" s="19"/>
-    </row>
-    <row r="70" spans="1:32" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:32" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="AE69" s="18">
+        <v>256</v>
+      </c>
+      <c r="AF69" s="8"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="8"/>
+      <c r="AI69" s="8"/>
+      <c r="AJ69" s="8"/>
+      <c r="AK69" s="8"/>
+      <c r="AL69" s="8"/>
+      <c r="AM69" s="8"/>
+      <c r="AN69" s="19"/>
+    </row>
+    <row r="70" spans="1:40" s="2" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:40" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="81" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="82" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="83" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -4420,7 +4962,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AA20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>

</xml_diff>